<commit_message>
Further development. Added kafka consumer Few Changes in Database table structure. Hence changes in JPA
</commit_message>
<xml_diff>
--- a/cashflow-consumer/src/main/resources/io/alw/css/cashflowconsumer/processor/rule/RevisionTypeResolver.drl.xlsx
+++ b/cashflow-consumer/src/main/resources/io/alw/css/cashflowconsumer/processor/rule/RevisionTypeResolver.drl.xlsx
@@ -26,7 +26,7 @@
     <t xml:space="preserve">RuleSet</t>
   </si>
   <si>
-    <t xml:space="preserve">io.alw.css.cashflowconsumer.mapper.rule</t>
+    <t xml:space="preserve">io.alw.css.cashflowconsumer.processor.rule</t>
   </si>
   <si>
     <t xml:space="preserve">Unit</t>
@@ -597,10 +597,10 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.88"/>
@@ -1183,7 +1183,7 @@
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.71"/>

</xml_diff>

<commit_message>
minor changes to debug and try to make drools work. Drools is NOT able to locate the rule spreadsheet file from within the jar. But drools does locate the rule spreadsheet file when running the unit test case. Exception is: java.lang.StringIndexOutOfBoundsException: Range [5, 3) out of bounds for length 164 	at java.base/java.lang.String.checkBoundsBeginEnd(String.java:4950) 	at java.base/java.lang.String.substring(String.java:2912) 	at org.drools.ruleunits.impl.RuleUnitProviderImpl.collectResourcesInJar(RuleUnitProviderImpl.java:192) 	at org.drools.ruleunits.impl.RuleUnitProviderImpl.ruleResourcesForUnitClass(RuleUnitProviderImpl.java:140)
</commit_message>
<xml_diff>
--- a/cashflow-consumer/src/main/resources/io/alw/css/cashflowconsumer/processor/rule/RevisionTypeResolver.drl.xlsx
+++ b/cashflow-consumer/src/main/resources/io/alw/css/cashflowconsumer/processor/rule/RevisionTypeResolver.drl.xlsx
@@ -597,10 +597,10 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.88"/>
@@ -1183,10 +1183,9 @@
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>